<commit_message>
Se crea Array, Split y Remove para quitar Colombian Pesos, y anexar Pesos Colombianos
</commit_message>
<xml_diff>
--- a/Resultado.xlsx
+++ b/Resultado.xlsx
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>4615,1405 Colombian Pesos</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>DÓLAR:</t>
   </si>
@@ -27,12 +24,6 @@
   </si>
   <si>
     <t xml:space="preserve">CANADIENCES: </t>
-  </si>
-  <si>
-    <t>4495,5474 Colombian Pesos</t>
-  </si>
-  <si>
-    <t>3356,252 Colombian Pesos</t>
   </si>
 </sst>
 </file>
@@ -68,8 +59,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -374,37 +366,37 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="33.44140625" customWidth="1"/>
+    <col min="2" max="2" width="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" s="1">
+        <v>46197879</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44990324</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>33615976</v>
       </c>
     </row>
   </sheetData>

</xml_diff>